<commit_message>
Tagging work, final pass missing
</commit_message>
<xml_diff>
--- a/Docs/Tagging/tags_manitobamuseum_jodie.xlsx
+++ b/Docs/Tagging/tags_manitobamuseum_jodie.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8025" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="First tagging" sheetId="1" r:id="rId1"/>
+    <sheet name="Refine Tags Jodie" sheetId="2" r:id="rId2"/>
+    <sheet name="Refine Tags Juan" sheetId="3" r:id="rId3"/>
+    <sheet name="Merged Tags" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Merged Tags'!$A$1:$H$10</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="163">
   <si>
     <t>IMG_0916</t>
   </si>
@@ -253,13 +257,265 @@
   </si>
   <si>
     <t>time line</t>
+  </si>
+  <si>
+    <t>ambient audio</t>
+  </si>
+  <si>
+    <t>guide - person</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>quote [text, author]</t>
+  </si>
+  <si>
+    <t>trivia</t>
+  </si>
+  <si>
+    <t>collage</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>artefacts</t>
+  </si>
+  <si>
+    <t>story</t>
+  </si>
+  <si>
+    <t>glass box</t>
+  </si>
+  <si>
+    <t>on wall</t>
+  </si>
+  <si>
+    <t>individual objects</t>
+  </si>
+  <si>
+    <t>fosil</t>
+  </si>
+  <si>
+    <t>moving objects</t>
+  </si>
+  <si>
+    <t>glass window</t>
+  </si>
+  <si>
+    <t>public display</t>
+  </si>
+  <si>
+    <t>artefact</t>
+  </si>
+  <si>
+    <t>timeline</t>
+  </si>
+  <si>
+    <t>on floor</t>
+  </si>
+  <si>
+    <t>picture collage</t>
+  </si>
+  <si>
+    <t>celebrity</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>individual legend</t>
+  </si>
+  <si>
+    <t>hexagonal shape</t>
+  </si>
+  <si>
+    <t>long text</t>
+  </si>
+  <si>
+    <t>front view</t>
+  </si>
+  <si>
+    <t>top view</t>
+  </si>
+  <si>
+    <t>full body</t>
+  </si>
+  <si>
+    <t>rocks</t>
+  </si>
+  <si>
+    <t>hanging</t>
+  </si>
+  <si>
+    <t>videos</t>
+  </si>
+  <si>
+    <t>color backgrounds</t>
+  </si>
+  <si>
+    <t>changing lighting</t>
+  </si>
+  <si>
+    <t>related to character</t>
+  </si>
+  <si>
+    <t>low-glass panel</t>
+  </si>
+  <si>
+    <t>main picture</t>
+  </si>
+  <si>
+    <t>animals</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>side view</t>
+  </si>
+  <si>
+    <t>no-legend</t>
+  </si>
+  <si>
+    <t>ball pointer</t>
+  </si>
+  <si>
+    <t>illustrative picture</t>
+  </si>
+  <si>
+    <t>context (historical)</t>
+  </si>
+  <si>
+    <t>artefact drawing</t>
+  </si>
+  <si>
+    <t>drawings</t>
+  </si>
+  <si>
+    <t>picture</t>
+  </si>
+  <si>
+    <t>audio guide</t>
+  </si>
+  <si>
+    <t>art work</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>wall map</t>
+  </si>
+  <si>
+    <t>drawing (map?)</t>
+  </si>
+  <si>
+    <t>individual legends</t>
+  </si>
+  <si>
+    <t>changing legends</t>
+  </si>
+  <si>
+    <t>context (scene description)</t>
+  </si>
+  <si>
+    <t>situated legend</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>context (theoretical)</t>
+  </si>
+  <si>
+    <t>located</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>objects</t>
+  </si>
+  <si>
+    <t>highlight on object</t>
+  </si>
+  <si>
+    <t>group name</t>
+  </si>
+  <si>
+    <t>dynamic graph</t>
+  </si>
+  <si>
+    <t>summarizing legend</t>
+  </si>
+  <si>
+    <t>terms</t>
+  </si>
+  <si>
+    <t>graspables</t>
+  </si>
+  <si>
+    <t>sculture</t>
+  </si>
+  <si>
+    <t>on pedestal</t>
+  </si>
+  <si>
+    <t>graphs</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>map legend</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>donor</t>
+  </si>
+  <si>
+    <t>text-on-glass</t>
+  </si>
+  <si>
+    <t>circular dispay</t>
+  </si>
+  <si>
+    <t>referenced legend</t>
+  </si>
+  <si>
+    <t>context (hist, scene, theor)</t>
+  </si>
+  <si>
+    <t>graph  (static, dynamic)</t>
+  </si>
+  <si>
+    <t>indexed label</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>no-label</t>
+  </si>
+  <si>
+    <t>summarizing label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +526,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -290,7 +553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -417,20 +680,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -452,6 +724,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,746 +1056,746 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="14"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="15"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="15"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="15"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="15"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="15"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="15"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="15"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="15"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="15"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="15"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="15"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="15"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="15"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="15"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H18" s="15"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="15"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="15"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="15"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="15"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="15"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="15"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="15"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="15"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="15"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="15"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H29" s="15"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="15"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="15"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="15"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="15"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H34" s="15"/>
+      <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="H35" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="16"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1524,24 +1808,908 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:B151">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A82"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A293">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="50.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:8" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="19"/>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A119">
+    <sortCondition ref="A49"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="54" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="4" max="9" man="1"/>
+  </colBreaks>
+</worksheet>
 </file>
</xml_diff>